<commit_message>
Banking project on spring and angular ui
In this project we are using Spring  data,boot ,security,web and in angular UI part HTML,CSS,Bootstrap,Javascript  .
</commit_message>
<xml_diff>
--- a/DxcTeam-4.xlsx
+++ b/DxcTeam-4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsahu27\Desktop\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08503233-D93A-418F-B3FA-BC7AB1BA2681}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2B596A-CF7A-408C-A890-91EC986190F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A0567C82-9405-482A-836E-AF27801280E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Email</t>
   </si>
@@ -103,13 +103,73 @@
   </si>
   <si>
     <t>Ministatement( Monthly , Annually)  &amp; Transfer Funds component</t>
+  </si>
+  <si>
+    <t>All Bank Representative Level Account Operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transfer Funds and help to desiging the homePage </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pay utility bills from IBS recognized service providers.</t>
+    </r>
+  </si>
+  <si>
+    <t>kritivardhan.singh@dxc.com</t>
+  </si>
+  <si>
+    <t>Remittance Management</t>
+  </si>
+  <si>
+    <t>ANGULAR UI PART:-</t>
+  </si>
+  <si>
+    <t>Remittance Management Part</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login And Registration &amp;  Pay utility bills from IBS </t>
+  </si>
+  <si>
+    <t>Transfer Fund Part</t>
+  </si>
+  <si>
+    <t>Working on both the validations and Account Opertions also</t>
+  </si>
+  <si>
+    <t>MIDDLE WARE PART:-</t>
+  </si>
+  <si>
+    <t>Request Mini Statement and Check Balance</t>
+  </si>
+  <si>
+    <t>Login And Registration &amp;  Check Balance</t>
+  </si>
+  <si>
+    <t>Integration and Validation both the  end</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +183,26 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -147,9 +227,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -465,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FDA8BDF-2EBE-4F21-A653-CF928608D2A8}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,7 +560,7 @@
     <col min="2" max="2" width="14.90625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="4" width="18.08984375" customWidth="1"/>
-    <col min="5" max="5" width="57.1796875" customWidth="1"/>
+    <col min="5" max="5" width="64.6328125" customWidth="1"/>
     <col min="6" max="6" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -598,6 +681,220 @@
       </c>
       <c r="E7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>11602542</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>11602433</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>11602441</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>11602544</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>11602424</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>11602429</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>11602542</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>11602433</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>11602441</v>
+      </c>
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>11602544</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>11602424</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>11602429</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -608,7 +905,20 @@
     <hyperlink ref="A5" r:id="rId4" xr:uid="{BA9D6EF6-E202-439B-BC17-A80AE4D2052D}"/>
     <hyperlink ref="A6" r:id="rId5" xr:uid="{86396416-20F0-4258-A02F-558B8DE34957}"/>
     <hyperlink ref="A7" r:id="rId6" xr:uid="{11166618-3E19-4CD3-81DD-A4A00DB8790E}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{AED0C060-6493-4288-9DB8-94A0DAE37432}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{97609E2E-3E2F-4411-AC64-7579843B669B}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{A5E09543-7F0A-463F-ACEF-1FEE1222DBFD}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{1FEF7744-8A50-40D8-8D6E-F58EBC21715F}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{B470C395-BA43-4D58-B8AC-EB389BEFAD2F}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{C3390D00-5766-475F-8230-7BDE085A9C34}"/>
+    <hyperlink ref="A18" r:id="rId13" xr:uid="{F25C3321-CB0B-413F-A35C-4747EF748B60}"/>
+    <hyperlink ref="A19" r:id="rId14" xr:uid="{5BC35F38-A331-4278-A897-8680FFA84CFC}"/>
+    <hyperlink ref="A20" r:id="rId15" xr:uid="{2B68166B-D20B-4F4E-90A8-6157A4871FA3}"/>
+    <hyperlink ref="A21" r:id="rId16" xr:uid="{0D7C9EA0-BE3F-4AFE-A1B5-65DE2D8A738B}"/>
+    <hyperlink ref="A22" r:id="rId17" xr:uid="{90107506-5799-40A1-8733-8091002C062B}"/>
+    <hyperlink ref="A23" r:id="rId18" xr:uid="{19BC14BF-4C3C-4AAF-B603-534BF3DE249F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>